<commit_message>
GOVT 2305 grades update
</commit_message>
<xml_diff>
--- a/1.2-GOVT-2305.003/Grades.xlsx
+++ b/1.2-GOVT-2305.003/Grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\UTDSpring2019\1.2-GOVT-2305.003\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871A48B6-F7AC-4A7A-91A5-A81289A36564}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FD99D5-9EA4-4407-A148-8C05070CEA14}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4830" windowWidth="28755" windowHeight="12840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -317,16 +317,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -675,7 +675,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,8 +687,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="24"/>
-      <c r="B1" s="24"/>
+      <c r="A1" s="27"/>
+      <c r="B1" s="27"/>
       <c r="C1" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -758,27 +758,27 @@
         <v>7</v>
       </c>
       <c r="C6" s="8">
-        <f>COUNT(C8:C23)</f>
+        <f t="shared" ref="C6:H6" si="0">COUNT(C8:C23)</f>
         <v>16</v>
       </c>
       <c r="D6" s="8">
-        <f>COUNT(D8:D23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E6" s="8">
-        <f>COUNT(E8:E23)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F6" s="8">
-        <f>COUNT(F8:F23)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="G6" s="8">
-        <f>COUNT(G8:G23)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H6" s="8">
-        <f>COUNT(H8:H23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I6" s="21"/>
@@ -792,33 +792,33 @@
         <v>13</v>
       </c>
       <c r="C7" s="16">
-        <f>IF(C6&lt;&gt;0,IF(C5&lt;&gt;0,(SUM(C8:C23)/C6)*C5,0), 0)</f>
+        <f t="shared" ref="C7:H7" si="1">IF(C6&lt;&gt;0,IF(C5&lt;&gt;0,(SUM(C8:C23)/C6)*C5,0), 0)</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D7" s="9">
-        <f>IF(D6&lt;&gt;0,IF(D5&lt;&gt;0,(SUM(D8:D23)/D6)*D5,0), 0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E7" s="9">
-        <f>IF(E6&lt;&gt;0,IF(E5&lt;&gt;0,(SUM(E8:E23)/E6)*E5,0), 0)</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="F7" s="9">
-        <f>IF(F6&lt;&gt;0,IF(F5&lt;&gt;0,(SUM(F8:F23)/F6)*F5,0), 0)</f>
-        <v>0.14000000000000001</v>
+        <f t="shared" si="1"/>
+        <v>0.13800000000000001</v>
       </c>
       <c r="G7" s="9">
-        <f>IF(G6&lt;&gt;0,IF(G5&lt;&gt;0,(SUM(G8:G23)/G6)*G5,0), 0)</f>
+        <f t="shared" si="1"/>
         <v>0.69</v>
       </c>
       <c r="H7" s="9">
-        <f>IF(H6&lt;&gt;0,IF(H5&lt;&gt;0,(SUM(H8:H23)/H6)*H5,0), 0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I7" s="21"/>
       <c r="J7" s="21">
         <f>SUM(C7:H7)</f>
-        <v>1</v>
+        <v>0.998</v>
       </c>
       <c r="K7" s="21"/>
       <c r="L7" s="5"/>
@@ -838,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="18">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G8" s="10">
         <v>1</v>
@@ -1087,7 +1087,7 @@
       <c r="L21" s="2"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="25">
+      <c r="B22" s="24">
         <v>15</v>
       </c>
       <c r="C22" s="17">
@@ -1103,10 +1103,10 @@
       <c r="K22" s="21"/>
     </row>
     <row r="23" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="26">
+      <c r="B23" s="25">
         <v>16</v>
       </c>
-      <c r="C23" s="27">
+      <c r="C23" s="26">
         <v>1</v>
       </c>
       <c r="D23" s="13"/>

</xml_diff>

<commit_message>
doc 9 notes started
</commit_message>
<xml_diff>
--- a/1.2-GOVT-2305.003/Grades.xlsx
+++ b/1.2-GOVT-2305.003/Grades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\UTDSpring2019\1.2-GOVT-2305.003\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEE703B-B4B0-4F73-A7FC-F7A255921067}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8282E5F8-F7E6-4859-A07B-C576E1E91BC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="1950" windowWidth="24345" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6420" yWindow="825" windowWidth="20610" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -654,7 +654,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,11 +784,11 @@
       </c>
       <c r="F7" s="7">
         <f t="shared" si="1"/>
-        <v>0.13131999999999999</v>
+        <v>0.12132000000000001</v>
       </c>
       <c r="G7" s="7">
         <f t="shared" si="1"/>
-        <v>0.50024999999999997</v>
+        <v>0.47150000000000003</v>
       </c>
       <c r="H7" s="7">
         <f t="shared" si="1"/>
@@ -797,7 +797,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1">
         <f>SUM(C7:H7)</f>
-        <v>0.79657</v>
+        <v>0.75782000000000005</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -841,7 +841,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="10">
-        <v>0.7</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="1"/>
@@ -862,7 +862,7 @@
         <v>0.66600000000000004</v>
       </c>
       <c r="G10" s="10">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="1"/>
@@ -918,7 +918,7 @@
       <c r="D13" s="15"/>
       <c r="E13" s="10"/>
       <c r="F13" s="17">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>

</xml_diff>